<commit_message>
added new exception into main script for establishing driver session
</commit_message>
<xml_diff>
--- a/HL7_parsor/KAISER PERMANENTE REGIONAL REFERENCE LAB _ CHINO HILLS CDPH/Urine Culture_ACCnum_000022023268009304_DInum_4211306.xlsx
+++ b/HL7_parsor/KAISER PERMANENTE REGIONAL REFERENCE LAB _ CHINO HILLS CDPH/Urine Culture_ACCnum_000022023268009304_DInum_4211306.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sdcountycagov-my.sharepoint.com/personal/kiarash_rastegar_sdcounty_ca_gov/Documents/Desktop/TST_WebAutomation/HL7_parsor/KAISER PERMANENTE REGIONAL REFERENCE LAB _ CHINO HILLS CDPH/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2BB1D69C5B70D3467B7B3611590560B767DFEA1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3B6FF8B-56EE-4EF3-AC01-7C119B8D7230}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_2BB1D69C5BD0511ABF3B3411590560B767DFEA1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9E359E8-04C8-452C-B62B-56FA71A7CCA2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -667,7 +667,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>